<commit_message>
deal with security implementation in the backend
</commit_message>
<xml_diff>
--- a/Programme de travail/Programme.xlsx
+++ b/Programme de travail/Programme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projet Mobile\Application Mobile Système de vote par Internet\Programme de travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45F490F-C431-44FB-A857-49C375AA6892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2AFCB2-0D35-40CE-B3F9-2B8E81748C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13023" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,10 +42,10 @@
     <t>Spring Security</t>
   </si>
   <si>
-    <t>Login Flutter/ UI + Link</t>
-  </si>
-  <si>
     <t>UI /UX</t>
+  </si>
+  <si>
+    <t>Spring Services</t>
   </si>
 </sst>
 </file>
@@ -406,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E7:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="127" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="G3" zoomScale="127" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -415,6 +415,7 @@
     <col min="5" max="5" width="31.21875" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="28.6640625" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="5:8" ht="37.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -452,7 +453,7 @@
     </row>
     <row r="10" spans="5:8" ht="39.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E10" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F10" s="3">
         <v>45409</v>
@@ -464,7 +465,7 @@
     </row>
     <row r="11" spans="5:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>

</xml_diff>